<commit_message>
final code before changing to zeroinfl()
</commit_message>
<xml_diff>
--- a/Observations by field assistants.xlsx
+++ b/Observations by field assistants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Library/Mobile Documents/com~apple~CloudDocs/Agribirds Sweden iCloud/stats/AgriBirds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB129D55-38DB-2446-8E2D-5228064991C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9CB042-3624-694E-BF11-46DE9353BA0E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-5600" windowWidth="38400" windowHeight="21600" xr2:uid="{4DC26ADA-6801-4546-89A8-C076626D53A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{4DC26ADA-6801-4546-89A8-C076626D53A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="37">
   <si>
     <t>objectID</t>
   </si>
@@ -119,12 +114,6 @@
     <t>distcc</t>
   </si>
   <si>
-    <t>farmland_250</t>
-  </si>
-  <si>
-    <t>clearcuts250</t>
-  </si>
-  <si>
     <t>propfl_250</t>
   </si>
   <si>
@@ -141,6 +130,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>clear-cut</t>
   </si>
 </sst>
 </file>
@@ -498,15 +493,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B335332-9DF6-B448-BB7A-1D909B249673}">
-  <dimension ref="A1:AG32"/>
+  <dimension ref="A1:AE31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="16" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,136 +600,184 @@
       <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
+    </row>
+    <row r="2" spans="1:31">
+      <c r="A2">
+        <v>1009433</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43265</v>
+      </c>
+      <c r="F2">
+        <v>10.45</v>
+      </c>
+      <c r="G2">
+        <v>4070</v>
+      </c>
+      <c r="H2" s="1">
+        <v>41472</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
         <v>32</v>
       </c>
+      <c r="K2">
+        <v>35</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+      <c r="O2">
+        <v>25</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <f t="shared" ref="S2:S31" si="0">SUM(K2:R2)</f>
+        <v>100</v>
+      </c>
+      <c r="T2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>116.396770694696</v>
+      </c>
+      <c r="AE2">
+        <v>4.9000000000000002E-2</v>
+      </c>
     </row>
-    <row r="2" spans="1:33">
-      <c r="A2">
-        <v>1590416</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>43269</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.43055555555555558</v>
-      </c>
-      <c r="I2" t="s">
+    <row r="3" spans="1:31">
+      <c r="A3">
+        <v>1019378</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43272</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.34513888888888888</v>
+      </c>
+      <c r="G3">
+        <v>17073</v>
+      </c>
+      <c r="H3" s="1">
+        <v>41472</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3">
         <v>33</v>
       </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>5</v>
-      </c>
-      <c r="M2">
-        <v>9</v>
-      </c>
-      <c r="N2">
-        <v>17</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>9</v>
-      </c>
-      <c r="Q2">
-        <v>9</v>
-      </c>
-      <c r="R2">
-        <v>51</v>
-      </c>
-      <c r="S2">
-        <f>SUM(K2:R2)</f>
+      <c r="L3">
+        <v>32</v>
+      </c>
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="N3">
+        <v>24</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="T2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" t="s">
-        <v>36</v>
+      <c r="T3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" t="s">
+        <v>31</v>
+      </c>
+      <c r="X3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>232.938363908284</v>
+      </c>
+      <c r="AE3">
+        <v>2E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3">
-        <v>1009433</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>43265</v>
-      </c>
-      <c r="F3">
-        <v>10.45</v>
-      </c>
-      <c r="I3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3">
-        <v>35</v>
-      </c>
-      <c r="L3">
-        <v>5</v>
-      </c>
-      <c r="M3">
-        <v>5</v>
-      </c>
-      <c r="N3">
-        <v>30</v>
-      </c>
-      <c r="O3">
-        <v>25</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <f t="shared" ref="S3:S32" si="0">SUM(K3:R3)</f>
-        <v>100</v>
-      </c>
-      <c r="T3" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="4">
-        <v>1736915</v>
+    <row r="4" spans="1:31">
+      <c r="A4">
+        <v>1208249</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -738,118 +786,172 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>43265</v>
+        <v>43275</v>
       </c>
       <c r="F4" s="3">
-        <v>0.4861111111111111</v>
+        <v>0.40625</v>
+      </c>
+      <c r="G4">
+        <v>8515</v>
+      </c>
+      <c r="H4" s="1">
+        <v>41845</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K4">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>50</v>
+      </c>
+      <c r="O4">
         <v>2</v>
       </c>
-      <c r="M4">
-        <v>15</v>
-      </c>
-      <c r="N4">
-        <v>3</v>
-      </c>
-      <c r="O4">
-        <v>5</v>
-      </c>
       <c r="P4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Q4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="R4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="T4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W4" t="s">
         <v>36</v>
       </c>
+      <c r="X4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>8.3531995532855507</v>
+      </c>
+      <c r="AE4">
+        <v>9.7000000000000003E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:31">
       <c r="A5">
-        <v>1822983</v>
+        <v>1452122</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>43270</v>
+        <v>43272</v>
       </c>
       <c r="F5" s="3">
-        <v>0.50555555555555554</v>
+        <v>0.46319444444444446</v>
+      </c>
+      <c r="G5">
+        <v>16940</v>
+      </c>
+      <c r="H5" s="1">
+        <v>42255</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K5">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>25</v>
+      </c>
+      <c r="N5">
         <v>10</v>
       </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
-      <c r="N5">
-        <v>5</v>
-      </c>
       <c r="O5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="P5">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="T5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y5" t="s">
         <v>36</v>
       </c>
-      <c r="U5" t="s">
-        <v>36</v>
+      <c r="Z5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:31">
       <c r="A6">
-        <v>1575284</v>
+        <v>1454595</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -861,34 +963,40 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>43271</v>
+        <v>43291</v>
       </c>
       <c r="F6" s="3">
-        <v>0.40833333333333338</v>
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="G6">
+        <v>6374</v>
+      </c>
+      <c r="H6" s="1">
+        <v>42166</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K6">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N6">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="O6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="P6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -901,15 +1009,39 @@
         <v>100</v>
       </c>
       <c r="T6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="U6" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="V6">
+        <v>2</v>
+      </c>
+      <c r="W6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA6">
+        <v>0.5</v>
+      </c>
+      <c r="AC6">
+        <v>229.88344384860801</v>
+      </c>
+      <c r="AE6">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:31">
       <c r="A7">
-        <v>1736794</v>
+        <v>1470704</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -921,61 +1053,88 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>43271</v>
+        <v>43276</v>
       </c>
       <c r="F7" s="3">
-        <v>10.38</v>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G7">
+        <v>3129</v>
+      </c>
+      <c r="H7" s="1">
+        <v>42255</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L7">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="M7">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="P7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="Q7">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="T7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="U7" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="W7" t="s">
+        <v>31</v>
+      </c>
+      <c r="X7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <v>151.16350990444701</v>
+      </c>
+      <c r="AE7">
+        <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:31">
       <c r="A8">
-        <v>1736705</v>
+        <v>1496659</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -984,154 +1143,214 @@
         <v>43271</v>
       </c>
       <c r="F8" s="3">
-        <v>0.50208333333333333</v>
+        <v>0.49791666666666662</v>
+      </c>
+      <c r="G8">
+        <v>16169</v>
+      </c>
+      <c r="H8" s="1">
+        <v>41829</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K8">
+        <v>22</v>
+      </c>
+      <c r="L8">
         <v>15</v>
       </c>
-      <c r="L8">
+      <c r="M8">
+        <v>15</v>
+      </c>
+      <c r="N8">
+        <v>35</v>
+      </c>
+      <c r="O8">
         <v>10</v>
       </c>
-      <c r="M8">
-        <v>20</v>
-      </c>
-      <c r="N8">
-        <v>5</v>
-      </c>
-      <c r="O8">
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
         <v>2</v>
-      </c>
-      <c r="P8">
-        <v>28</v>
-      </c>
-      <c r="Q8">
-        <v>5</v>
-      </c>
-      <c r="R8">
-        <v>15</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="T8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="U8" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="W8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA8">
+        <v>0.75</v>
+      </c>
+      <c r="AC8">
+        <v>40.480399734028801</v>
+      </c>
+      <c r="AE8">
+        <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:31">
       <c r="A9">
-        <v>1736699</v>
+        <v>1497782</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1">
-        <v>43271</v>
+        <v>43272</v>
       </c>
       <c r="F9" s="3">
-        <v>0.52500000000000002</v>
+        <v>0.39861111111111108</v>
+      </c>
+      <c r="G9">
+        <v>11059</v>
+      </c>
+      <c r="H9" s="1">
+        <v>41829</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K9">
+        <v>15</v>
+      </c>
+      <c r="L9">
+        <v>35</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
         <v>40</v>
       </c>
-      <c r="L9">
-        <v>3</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>10</v>
-      </c>
       <c r="O9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P9">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R9">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="T9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W9" t="s">
         <v>36</v>
       </c>
-      <c r="U9" t="s">
+      <c r="X9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y9" t="s">
         <v>36</v>
       </c>
+      <c r="Z9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA9">
+        <v>0.25</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0.106</v>
+      </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:31">
       <c r="A10">
-        <v>1019378</v>
+        <v>1501339</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>43278</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="G10">
+        <v>11587</v>
+      </c>
+      <c r="H10" s="1">
+        <v>42255</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10">
+        <v>65</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
         <v>3</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>43272</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.34513888888888888</v>
-      </c>
-      <c r="I10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10">
-        <v>33</v>
-      </c>
-      <c r="L10">
-        <v>32</v>
-      </c>
-      <c r="M10">
-        <v>5</v>
-      </c>
       <c r="N10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="P10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -1140,10 +1359,37 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T10" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10" t="s">
+        <v>34</v>
+      </c>
+      <c r="W10" t="s">
+        <v>31</v>
+      </c>
+      <c r="X10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA10">
+        <v>0.5</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0.10299999999999999</v>
+      </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:31">
       <c r="A11">
-        <v>1497782</v>
+        <v>1524607</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1152,106 +1398,172 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>43272</v>
+        <v>43277</v>
       </c>
       <c r="F11" s="3">
-        <v>0.39861111111111108</v>
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="G11">
+        <v>43027</v>
+      </c>
+      <c r="H11" s="1">
+        <v>42255</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K11">
+        <v>20</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <v>7</v>
+      </c>
+      <c r="N11">
         <v>15</v>
       </c>
-      <c r="L11">
+      <c r="O11">
+        <v>8</v>
+      </c>
+      <c r="P11">
+        <v>5</v>
+      </c>
+      <c r="Q11">
         <v>35</v>
       </c>
-      <c r="M11">
-        <v>2</v>
-      </c>
-      <c r="N11">
-        <v>40</v>
-      </c>
-      <c r="O11">
-        <v>5</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>2</v>
-      </c>
       <c r="R11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S11">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T11" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" t="s">
+        <v>34</v>
+      </c>
+      <c r="W11" t="s">
+        <v>31</v>
+      </c>
+      <c r="X11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA11">
+        <v>0.5</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>4.8000000000000001E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:31">
       <c r="A12">
-        <v>1736691</v>
+        <v>1525828</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>43275</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="G12">
+        <v>41974</v>
+      </c>
+      <c r="H12" s="1">
+        <v>42255</v>
+      </c>
+      <c r="I12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12">
+        <v>50</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
         <v>2</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>43264</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="I12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12">
-        <v>49</v>
-      </c>
-      <c r="L12">
-        <v>8</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
       <c r="N12">
+        <v>5</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+      <c r="P12">
+        <v>10</v>
+      </c>
+      <c r="Q12">
         <v>15</v>
       </c>
-      <c r="O12">
-        <v>20</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>5</v>
-      </c>
       <c r="R12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S12">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T12" t="s">
+        <v>34</v>
+      </c>
+      <c r="U12" t="s">
+        <v>34</v>
+      </c>
+      <c r="W12" t="s">
+        <v>31</v>
+      </c>
+      <c r="X12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AC12">
+        <v>81.906172217320304</v>
+      </c>
+      <c r="AE12">
+        <v>0.129</v>
+      </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:31">
       <c r="A13">
-        <v>1539378</v>
+        <v>1538444</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1260,52 +1572,85 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1">
         <v>43270</v>
       </c>
       <c r="F13" s="3">
-        <v>0.38819444444444445</v>
+        <v>0.44166666666666665</v>
+      </c>
+      <c r="G13">
+        <v>9842</v>
+      </c>
+      <c r="H13" s="1">
+        <v>42166</v>
       </c>
       <c r="I13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K13">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M13">
+        <v>8</v>
+      </c>
+      <c r="N13">
         <v>45</v>
       </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
       <c r="O13">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="P13">
         <v>5</v>
       </c>
       <c r="Q13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T13" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13" t="s">
+        <v>34</v>
+      </c>
+      <c r="W13" t="s">
+        <v>35</v>
+      </c>
+      <c r="X13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA13">
+        <v>0.25</v>
+      </c>
+      <c r="AC13">
+        <v>43.852965812974602</v>
+      </c>
+      <c r="AE13">
+        <v>9.5000000000000001E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:31">
       <c r="A14">
-        <v>1538444</v>
+        <v>1539378</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1314,148 +1659,220 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="1">
         <v>43270</v>
       </c>
       <c r="F14" s="3">
-        <v>0.44166666666666665</v>
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="G14">
+        <v>18276</v>
+      </c>
+      <c r="H14" s="1">
+        <v>42166</v>
       </c>
       <c r="I14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>45</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>20</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+      <c r="Q14">
         <v>2</v>
       </c>
-      <c r="M14">
-        <v>8</v>
-      </c>
-      <c r="N14">
-        <v>45</v>
-      </c>
-      <c r="O14">
-        <v>25</v>
-      </c>
-      <c r="P14">
-        <v>5</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
       <c r="R14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S14">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T14" t="s">
+        <v>34</v>
+      </c>
+      <c r="U14" t="s">
+        <v>34</v>
+      </c>
+      <c r="W14" t="s">
+        <v>36</v>
+      </c>
+      <c r="X14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0.22600000000000001</v>
+      </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:31">
       <c r="A15">
-        <v>1501339</v>
+        <v>1574771</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>43276</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="G15">
+        <v>11751</v>
+      </c>
+      <c r="H15" s="1">
+        <v>42572</v>
+      </c>
+      <c r="I15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15">
+        <v>40</v>
+      </c>
+      <c r="L15">
+        <v>10</v>
+      </c>
+      <c r="M15">
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <v>20</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="P15">
         <v>4</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>43278</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.36805555555555558</v>
-      </c>
-      <c r="I15" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15">
-        <v>65</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>3</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>20</v>
-      </c>
-      <c r="P15">
-        <v>7</v>
-      </c>
       <c r="Q15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R15">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="S15">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T15" t="s">
+        <v>34</v>
+      </c>
+      <c r="U15" t="s">
+        <v>34</v>
+      </c>
+      <c r="W15" t="s">
+        <v>31</v>
+      </c>
+      <c r="X15" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>160.779293395731</v>
+      </c>
+      <c r="AE15">
+        <v>5.0999999999999997E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:31">
       <c r="A16">
-        <v>1452122</v>
+        <v>1574805</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>43272</v>
+        <v>43271</v>
       </c>
       <c r="F16" s="3">
-        <v>0.46319444444444446</v>
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="G16">
+        <v>24148</v>
+      </c>
+      <c r="H16" s="1">
+        <v>42572</v>
       </c>
       <c r="I16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K16">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L16">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M16">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="N16">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="O16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16">
         <v>1</v>
@@ -1464,10 +1881,37 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T16" t="s">
+        <v>34</v>
+      </c>
+      <c r="U16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W16" t="s">
+        <v>31</v>
+      </c>
+      <c r="X16" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA16">
+        <v>0.5</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0.109</v>
+      </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:31">
       <c r="A17">
-        <v>1736893</v>
+        <v>1574941</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1479,37 +1923,43 @@
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>43270</v>
+        <v>43291</v>
       </c>
       <c r="F17" s="3">
-        <v>0.5</v>
+        <v>0.51180555555555551</v>
+      </c>
+      <c r="G17">
+        <v>11380</v>
+      </c>
+      <c r="H17" s="1">
+        <v>42572</v>
       </c>
       <c r="I17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K17">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="L17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="N17">
         <v>30</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R17">
         <v>3</v>
@@ -1518,10 +1968,40 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T17" t="s">
+        <v>34</v>
+      </c>
+      <c r="U17" t="s">
+        <v>34</v>
+      </c>
+      <c r="V17">
+        <v>1.5</v>
+      </c>
+      <c r="W17" t="s">
+        <v>31</v>
+      </c>
+      <c r="X17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA17">
+        <v>0.5</v>
+      </c>
+      <c r="AC17">
+        <v>25.1189739622315</v>
+      </c>
+      <c r="AE17">
+        <v>6.3E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:31">
       <c r="A18">
-        <v>1574805</v>
+        <v>1575284</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1530,163 +2010,262 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
         <v>43271</v>
       </c>
       <c r="F18" s="3">
-        <v>0.4201388888888889</v>
+        <v>0.40833333333333338</v>
+      </c>
+      <c r="G18">
+        <v>6932</v>
+      </c>
+      <c r="H18" s="1">
+        <v>42572</v>
       </c>
       <c r="I18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K18">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="L18">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M18">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N18">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P18">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T18" t="s">
+        <v>34</v>
+      </c>
+      <c r="U18" t="s">
+        <v>34</v>
+      </c>
+      <c r="W18" t="s">
+        <v>31</v>
+      </c>
+      <c r="X18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA18">
+        <v>0.75</v>
+      </c>
+      <c r="AC18">
+        <v>188.02272319123199</v>
+      </c>
+      <c r="AE18">
+        <v>2.1000000000000001E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:31">
       <c r="A19">
-        <v>1496659</v>
+        <v>1575782</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>43271</v>
+        <v>43291</v>
       </c>
       <c r="F19" s="3">
-        <v>0.49791666666666662</v>
+        <v>0.37916666666666665</v>
+      </c>
+      <c r="G19">
+        <v>10425</v>
+      </c>
+      <c r="H19" s="1">
+        <v>42572</v>
       </c>
       <c r="I19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K19">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="L19">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M19">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N19">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O19">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="P19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S19">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="T19" t="s">
+        <v>34</v>
+      </c>
+      <c r="U19" t="s">
+        <v>34</v>
+      </c>
+      <c r="V19">
+        <v>1.5</v>
+      </c>
+      <c r="W19" t="s">
+        <v>31</v>
+      </c>
+      <c r="X19" t="s">
         <v>35</v>
       </c>
+      <c r="Y19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA19">
+        <v>0.25</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>6.5000000000000002E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:31">
       <c r="A20">
-        <v>1501339</v>
+        <v>1590416</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>43271</v>
+        <v>43269</v>
       </c>
       <c r="F20" s="3">
-        <v>0.53472222222222221</v>
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="G20">
+        <v>9161</v>
+      </c>
+      <c r="H20" s="1">
+        <v>42572</v>
       </c>
       <c r="I20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N20">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O20">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P20">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="Q20">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="R20">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="S20">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T20" t="s">
+        <v>34</v>
+      </c>
+      <c r="U20" t="s">
+        <v>34</v>
+      </c>
+      <c r="W20" t="s">
+        <v>31</v>
+      </c>
+      <c r="X20" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA20">
+        <v>0.75</v>
+      </c>
+      <c r="AC20">
+        <v>12.5828668778456</v>
+      </c>
+      <c r="AE20">
+        <v>7.4999999999999997E-2</v>
+      </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:31">
       <c r="A21">
-        <v>1208249</v>
+        <v>1592218</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1695,217 +2274,349 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>43275</v>
+        <v>43287</v>
       </c>
       <c r="F21" s="3">
-        <v>0.40625</v>
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="G21">
+        <v>7549</v>
+      </c>
+      <c r="H21" s="1">
+        <v>42572</v>
       </c>
       <c r="I21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K21">
+        <v>22</v>
+      </c>
+      <c r="L21">
+        <v>5</v>
+      </c>
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <v>5</v>
+      </c>
+      <c r="O21">
+        <v>25</v>
+      </c>
+      <c r="P21">
+        <v>20</v>
+      </c>
+      <c r="Q21">
+        <v>8</v>
+      </c>
+      <c r="R21">
         <v>12</v>
-      </c>
-      <c r="L21">
-        <v>20</v>
-      </c>
-      <c r="M21">
-        <v>5</v>
-      </c>
-      <c r="N21">
-        <v>50</v>
-      </c>
-      <c r="O21">
-        <v>2</v>
-      </c>
-      <c r="P21">
-        <v>5</v>
-      </c>
-      <c r="Q21">
-        <v>5</v>
-      </c>
-      <c r="R21">
-        <v>1</v>
       </c>
       <c r="S21">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T21" t="s">
+        <v>34</v>
+      </c>
+      <c r="U21" t="s">
+        <v>34</v>
+      </c>
+      <c r="V21">
+        <v>0.4</v>
+      </c>
+      <c r="W21" t="s">
+        <v>36</v>
+      </c>
+      <c r="X21" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA21">
+        <v>0.5</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0.13200000000000001</v>
+      </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:31">
       <c r="A22">
-        <v>1525828</v>
+        <v>1659419</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>43275</v>
+        <v>43276</v>
       </c>
       <c r="F22" s="3">
-        <v>0.46875</v>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="G22">
+        <v>5328</v>
+      </c>
+      <c r="H22" s="1">
+        <v>42572</v>
       </c>
       <c r="I22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K22">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="L22">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P22">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Q22">
+        <v>25</v>
+      </c>
+      <c r="R22">
         <v>15</v>
-      </c>
-      <c r="R22">
-        <v>3</v>
       </c>
       <c r="S22">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T22" t="s">
+        <v>34</v>
+      </c>
+      <c r="U22" t="s">
+        <v>34</v>
+      </c>
+      <c r="W22" t="s">
+        <v>31</v>
+      </c>
+      <c r="X22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA22">
+        <v>0.75</v>
+      </c>
+      <c r="AC22">
+        <v>192.24828182967201</v>
+      </c>
+      <c r="AE22">
+        <v>1.4E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:31">
       <c r="A23">
-        <v>1470704</v>
+        <v>1736691</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>43276</v>
+        <v>43264</v>
       </c>
       <c r="F23" s="3">
-        <v>0.44444444444444442</v>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="G23">
+        <v>48186</v>
+      </c>
+      <c r="H23" s="1">
+        <v>42882</v>
       </c>
       <c r="I23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K23">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="L23">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M23">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="N23">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="O23">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>5</v>
+      </c>
+      <c r="R23">
         <v>2</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>5</v>
       </c>
       <c r="S23">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="T23" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="U23" t="s">
+        <v>34</v>
+      </c>
+      <c r="W23" t="s">
+        <v>31</v>
+      </c>
+      <c r="X23" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA23">
+        <v>1</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:31">
       <c r="A24">
-        <v>1659419</v>
+        <v>1736699</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>43276</v>
+        <v>43271</v>
       </c>
       <c r="F24" s="3">
-        <v>0.47916666666666669</v>
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="G24">
+        <v>14151</v>
+      </c>
+      <c r="H24" s="1">
+        <v>42882</v>
       </c>
       <c r="I24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K24">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="L24">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P24">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Q24">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="R24">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="S24">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T24" t="s">
+        <v>34</v>
+      </c>
+      <c r="U24" t="s">
+        <v>34</v>
+      </c>
+      <c r="W24" t="s">
+        <v>31</v>
+      </c>
+      <c r="X24" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA24">
+        <v>1</v>
+      </c>
+      <c r="AC24">
+        <v>123.733706129138</v>
+      </c>
+      <c r="AE24">
+        <v>0.10100000000000001</v>
+      </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:31">
       <c r="A25">
-        <v>1574771</v>
+        <v>1736705</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1917,157 +2628,256 @@
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>43276</v>
+        <v>43271</v>
       </c>
       <c r="F25" s="3">
-        <v>0.38541666666666669</v>
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="G25">
+        <v>7059</v>
+      </c>
+      <c r="H25" s="1">
+        <v>42882</v>
       </c>
       <c r="I25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K25">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="L25">
         <v>10</v>
       </c>
       <c r="M25">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="N25">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="O25">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P25">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="Q25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R25">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="S25">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T25" t="s">
+        <v>34</v>
+      </c>
+      <c r="U25" t="s">
+        <v>34</v>
+      </c>
+      <c r="W25" t="s">
+        <v>36</v>
+      </c>
+      <c r="X25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA25">
+        <v>0.75</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0.16300000000000001</v>
+      </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:31">
       <c r="A26">
-        <v>1524607</v>
+        <v>1736794</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>43277</v>
+        <v>43271</v>
       </c>
       <c r="F26" s="3">
-        <v>0.37847222222222227</v>
+        <v>10.38</v>
+      </c>
+      <c r="G26">
+        <v>17981</v>
+      </c>
+      <c r="H26" s="1">
+        <v>42882</v>
       </c>
       <c r="I26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
+      <c r="M26">
+        <v>40</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>10</v>
+      </c>
+      <c r="Q26">
+        <v>25</v>
+      </c>
+      <c r="R26">
         <v>20</v>
-      </c>
-      <c r="L26">
-        <v>5</v>
-      </c>
-      <c r="M26">
-        <v>7</v>
-      </c>
-      <c r="N26">
-        <v>15</v>
-      </c>
-      <c r="O26">
-        <v>8</v>
-      </c>
-      <c r="P26">
-        <v>5</v>
-      </c>
-      <c r="Q26">
-        <v>35</v>
-      </c>
-      <c r="R26">
-        <v>5</v>
       </c>
       <c r="S26">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T26" t="s">
+        <v>34</v>
+      </c>
+      <c r="U26" t="s">
+        <v>34</v>
+      </c>
+      <c r="W26" t="s">
+        <v>36</v>
+      </c>
+      <c r="X26" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA26">
+        <v>0.75</v>
+      </c>
+      <c r="AC26">
+        <v>50.044047018050001</v>
+      </c>
+      <c r="AE26">
+        <v>9.8000000000000004E-2</v>
+      </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:31">
       <c r="A27">
-        <v>1736934</v>
+        <v>1736893</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>43246</v>
+        <v>43270</v>
       </c>
       <c r="F27" s="3">
-        <v>0.49652777777777773</v>
+        <v>0.5</v>
+      </c>
+      <c r="G27">
+        <v>18842</v>
+      </c>
+      <c r="H27" s="1">
+        <v>42882</v>
       </c>
       <c r="I27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K27">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="L27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N27">
+        <v>30</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>5</v>
+      </c>
+      <c r="Q27">
+        <v>8</v>
+      </c>
+      <c r="R27">
         <v>3</v>
-      </c>
-      <c r="O27">
-        <v>20</v>
-      </c>
-      <c r="P27">
-        <v>10</v>
-      </c>
-      <c r="Q27">
-        <v>15</v>
-      </c>
-      <c r="R27">
-        <v>5</v>
       </c>
       <c r="S27">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T27" t="s">
+        <v>34</v>
+      </c>
+      <c r="U27" t="s">
+        <v>34</v>
+      </c>
+      <c r="W27" t="s">
+        <v>31</v>
+      </c>
+      <c r="X27" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AC27">
+        <v>118.74744584350699</v>
+      </c>
+      <c r="AE27">
+        <v>5.8000000000000003E-2</v>
+      </c>
     </row>
-    <row r="28" spans="1:22">
-      <c r="A28">
-        <v>1575782</v>
+    <row r="28" spans="1:31">
+      <c r="A28" s="4">
+        <v>1736915</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2079,109 +2889,169 @@
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>43291</v>
+        <v>43265</v>
       </c>
       <c r="F28" s="3">
-        <v>0.37916666666666665</v>
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="G28">
+        <v>12204</v>
+      </c>
+      <c r="H28" s="1">
+        <v>42882</v>
       </c>
       <c r="I28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K28">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="L28">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M28">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N28">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="O28">
         <v>5</v>
       </c>
       <c r="P28">
+        <v>2</v>
+      </c>
+      <c r="Q28">
+        <v>15</v>
+      </c>
+      <c r="R28">
         <v>3</v>
-      </c>
-      <c r="Q28">
-        <v>2</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
       </c>
       <c r="S28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="V28">
-        <v>1.5</v>
+      <c r="T28" t="s">
+        <v>33</v>
+      </c>
+      <c r="U28" t="s">
+        <v>34</v>
+      </c>
+      <c r="W28" t="s">
+        <v>31</v>
+      </c>
+      <c r="X28" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AC28">
+        <v>132.388321597078</v>
+      </c>
+      <c r="AE28">
+        <v>3.9E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:31">
       <c r="A29">
-        <v>1824801</v>
+        <v>1736934</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>43291</v>
+        <v>43246</v>
       </c>
       <c r="F29" s="3">
-        <v>0.40763888888888888</v>
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="G29">
+        <v>5848</v>
+      </c>
+      <c r="H29" s="1">
+        <v>42882</v>
       </c>
       <c r="I29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K29">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N29">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="O29">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="P29">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q29">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="R29">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S29">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="V29">
-        <v>1.5</v>
+      <c r="T29" t="s">
+        <v>34</v>
+      </c>
+      <c r="U29" t="s">
+        <v>34</v>
+      </c>
+      <c r="W29" t="s">
+        <v>36</v>
+      </c>
+      <c r="X29" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA29">
+        <v>0.75</v>
+      </c>
+      <c r="AC29">
+        <v>0</v>
+      </c>
+      <c r="AE29">
+        <v>0.129</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:31">
       <c r="A30">
-        <v>1454595</v>
+        <v>1822983</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -2193,52 +3063,82 @@
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>43291</v>
+        <v>43270</v>
       </c>
       <c r="F30" s="3">
-        <v>0.4597222222222222</v>
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="G30">
+        <v>20525</v>
+      </c>
+      <c r="H30" s="1">
+        <v>42882</v>
       </c>
       <c r="I30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K30">
+        <v>50</v>
+      </c>
+      <c r="L30">
         <v>10</v>
-      </c>
-      <c r="L30">
-        <v>2</v>
       </c>
       <c r="M30">
         <v>3</v>
       </c>
       <c r="N30">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
         <v>15</v>
       </c>
-      <c r="P30">
-        <v>5</v>
-      </c>
       <c r="Q30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R30">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S30">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="V30">
-        <v>2</v>
+      <c r="T30" t="s">
+        <v>34</v>
+      </c>
+      <c r="U30" t="s">
+        <v>34</v>
+      </c>
+      <c r="W30" t="s">
+        <v>36</v>
+      </c>
+      <c r="X30" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA30">
+        <v>0.5</v>
+      </c>
+      <c r="AC30">
+        <v>1.2372045945088E-3</v>
+      </c>
+      <c r="AE30">
+        <v>0.13100000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:31">
       <c r="A31">
-        <v>1574941</v>
+        <v>1824801</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -2253,104 +3153,56 @@
         <v>43291</v>
       </c>
       <c r="F31" s="3">
-        <v>0.51180555555555551</v>
+        <v>0.40763888888888888</v>
       </c>
       <c r="I31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K31">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L31">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M31">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="N31">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="O31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S31">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="T31" t="s">
+        <v>34</v>
+      </c>
+      <c r="U31" t="s">
+        <v>34</v>
+      </c>
       <c r="V31">
         <v>1.5</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
-      <c r="A32">
-        <v>1592218</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
-        <v>43287</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0.38541666666666669</v>
-      </c>
-      <c r="I32" t="s">
-        <v>33</v>
-      </c>
-      <c r="J32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K32">
-        <v>22</v>
-      </c>
-      <c r="L32">
-        <v>5</v>
-      </c>
-      <c r="M32">
-        <v>3</v>
-      </c>
-      <c r="N32">
-        <v>5</v>
-      </c>
-      <c r="O32">
-        <v>25</v>
-      </c>
-      <c r="P32">
-        <v>20</v>
-      </c>
-      <c r="Q32">
-        <v>8</v>
-      </c>
-      <c r="R32">
-        <v>12</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="V32">
-        <v>0.4</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:AE31">
+    <sortCondition ref="A2:A31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New agri dist calculations, backup of script
</commit_message>
<xml_diff>
--- a/Observations by field assistants.xlsx
+++ b/Observations by field assistants.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Library/Mobile Documents/com~apple~CloudDocs/Agribirds Sweden iCloud/stats/AgriBirds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9CB042-3624-694E-BF11-46DE9353BA0E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60CE272-71C2-BE4B-93F5-90C6870942D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{4DC26ADA-6801-4546-89A8-C076626D53A2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{4DC26ADA-6801-4546-89A8-C076626D53A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -493,17 +498,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B335332-9DF6-B448-BB7A-1D909B249673}">
-  <dimension ref="A1:AE31"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W31" sqref="W31"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="16" width="10.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -666,6 +683,9 @@
       <c r="U2" t="s">
         <v>33</v>
       </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
       <c r="W2" t="s">
         <v>31</v>
       </c>
@@ -753,6 +773,9 @@
       <c r="U3" t="s">
         <v>34</v>
       </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
       <c r="W3" t="s">
         <v>31</v>
       </c>
@@ -840,6 +863,9 @@
       <c r="U4" t="s">
         <v>34</v>
       </c>
+      <c r="V4">
+        <v>1.5</v>
+      </c>
       <c r="W4" t="s">
         <v>36</v>
       </c>
@@ -927,6 +953,9 @@
       <c r="U5" t="s">
         <v>34</v>
       </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
       <c r="W5" t="s">
         <v>35</v>
       </c>
@@ -1104,6 +1133,9 @@
       <c r="U7" t="s">
         <v>34</v>
       </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
       <c r="W7" t="s">
         <v>31</v>
       </c>
@@ -1191,6 +1223,9 @@
       <c r="U8" t="s">
         <v>34</v>
       </c>
+      <c r="V8">
+        <v>1.2</v>
+      </c>
       <c r="W8" t="s">
         <v>31</v>
       </c>
@@ -1278,6 +1313,9 @@
       <c r="U9" t="s">
         <v>34</v>
       </c>
+      <c r="V9">
+        <v>2</v>
+      </c>
       <c r="W9" t="s">
         <v>36</v>
       </c>
@@ -1452,6 +1490,9 @@
       <c r="U11" t="s">
         <v>34</v>
       </c>
+      <c r="V11">
+        <v>0.2</v>
+      </c>
       <c r="W11" t="s">
         <v>31</v>
       </c>
@@ -1539,6 +1580,9 @@
       <c r="U12" t="s">
         <v>34</v>
       </c>
+      <c r="V12">
+        <v>0.5</v>
+      </c>
       <c r="W12" t="s">
         <v>31</v>
       </c>
@@ -1626,6 +1670,9 @@
       <c r="U13" t="s">
         <v>34</v>
       </c>
+      <c r="V13">
+        <v>1.5</v>
+      </c>
       <c r="W13" t="s">
         <v>35</v>
       </c>
@@ -1713,6 +1760,9 @@
       <c r="U14" t="s">
         <v>34</v>
       </c>
+      <c r="V14">
+        <v>1.5</v>
+      </c>
       <c r="W14" t="s">
         <v>36</v>
       </c>
@@ -1800,6 +1850,9 @@
       <c r="U15" t="s">
         <v>34</v>
       </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
       <c r="W15" t="s">
         <v>31</v>
       </c>
@@ -1887,6 +1940,9 @@
       <c r="U16" t="s">
         <v>34</v>
       </c>
+      <c r="V16">
+        <v>2</v>
+      </c>
       <c r="W16" t="s">
         <v>31</v>
       </c>
@@ -2064,6 +2120,9 @@
       <c r="U18" t="s">
         <v>34</v>
       </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
       <c r="W18" t="s">
         <v>31</v>
       </c>
@@ -2241,6 +2300,9 @@
       <c r="U20" t="s">
         <v>34</v>
       </c>
+      <c r="V20">
+        <v>0.5</v>
+      </c>
       <c r="W20" t="s">
         <v>31</v>
       </c>
@@ -2418,6 +2480,9 @@
       <c r="U22" t="s">
         <v>34</v>
       </c>
+      <c r="V22">
+        <v>1.5</v>
+      </c>
       <c r="W22" t="s">
         <v>31</v>
       </c>
@@ -2592,6 +2657,9 @@
       <c r="U24" t="s">
         <v>34</v>
       </c>
+      <c r="V24">
+        <v>0.5</v>
+      </c>
       <c r="W24" t="s">
         <v>31</v>
       </c>
@@ -2679,6 +2747,9 @@
       <c r="U25" t="s">
         <v>34</v>
       </c>
+      <c r="V25">
+        <v>0.2</v>
+      </c>
       <c r="W25" t="s">
         <v>36</v>
       </c>
@@ -2766,6 +2837,9 @@
       <c r="U26" t="s">
         <v>34</v>
       </c>
+      <c r="V26">
+        <v>0.4</v>
+      </c>
       <c r="W26" t="s">
         <v>36</v>
       </c>
@@ -2853,6 +2927,9 @@
       <c r="U27" t="s">
         <v>34</v>
       </c>
+      <c r="V27">
+        <v>0.5</v>
+      </c>
       <c r="W27" t="s">
         <v>31</v>
       </c>
@@ -3027,6 +3104,9 @@
       <c r="U29" t="s">
         <v>34</v>
       </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
       <c r="W29" t="s">
         <v>36</v>
       </c>
@@ -3114,6 +3194,9 @@
       <c r="U30" t="s">
         <v>34</v>
       </c>
+      <c r="V30">
+        <v>0.2</v>
+      </c>
       <c r="W30" t="s">
         <v>36</v>
       </c>
@@ -3198,6 +3281,12 @@
       <c r="V31">
         <v>1.5</v>
       </c>
+    </row>
+    <row r="32" spans="1:31">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:AE31">

</xml_diff>